<commit_message>
update return status when import duplicate
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/Template_Import_Syllabus.xlsx
+++ b/src/main/resources/templates/Template_Import_Syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSA\Project\fms-backend-api\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1288C0CB-C690-4188-9686-F8FD6BB9DC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5D4FFC-735B-4545-910D-BB24F1142922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -375,7 +375,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="175">
   <si>
     <t>Topic Name</t>
   </si>
@@ -971,6 +971,9 @@
   </si>
   <si>
     <t>TEEST</t>
+  </si>
+  <si>
+    <t>4.1</t>
   </si>
 </sst>
 </file>
@@ -1855,26 +1858,26 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -2907,7 +2910,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:F5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
@@ -2984,8 +2987,8 @@
       <c r="B5" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="115">
-        <v>49</v>
+      <c r="C5" s="115" t="s">
+        <v>174</v>
       </c>
       <c r="D5" s="116"/>
       <c r="E5" s="116"/>
@@ -3377,23 +3380,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36.75" customHeight="1">
-      <c r="A1" s="124" t="str">
+      <c r="A1" s="122" t="str">
         <f>Syllabus!C3 &amp; " - Training Schedule"</f>
         <v>TEST - Training Schedule</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
     </row>
     <row r="2" spans="1:8" ht="39" customHeight="1">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="126"/>
+      <c r="B2" s="124"/>
       <c r="C2" s="31" t="s">
         <v>13</v>
       </c>
@@ -3417,7 +3420,7 @@
       <c r="A3" s="118">
         <v>1</v>
       </c>
-      <c r="B3" s="121" t="s">
+      <c r="B3" s="120" t="s">
         <v>81</v>
       </c>
       <c r="C3" s="34" t="s">
@@ -3441,7 +3444,7 @@
     </row>
     <row r="4" spans="1:8" ht="79.2">
       <c r="A4" s="119"/>
-      <c r="B4" s="122"/>
+      <c r="B4" s="121"/>
       <c r="C4" s="5" t="s">
         <v>84</v>
       </c>
@@ -3463,7 +3466,7 @@
     </row>
     <row r="5" spans="1:8" ht="79.2">
       <c r="A5" s="119"/>
-      <c r="B5" s="122"/>
+      <c r="B5" s="121"/>
       <c r="C5" s="39" t="s">
         <v>85</v>
       </c>
@@ -3485,7 +3488,7 @@
     </row>
     <row r="6" spans="1:8" ht="26.4">
       <c r="A6" s="119"/>
-      <c r="B6" s="122"/>
+      <c r="B6" s="121"/>
       <c r="C6" s="39" t="s">
         <v>86</v>
       </c>
@@ -3507,7 +3510,7 @@
     </row>
     <row r="7" spans="1:8" ht="158.4">
       <c r="A7" s="119"/>
-      <c r="B7" s="122"/>
+      <c r="B7" s="121"/>
       <c r="C7" s="40" t="s">
         <v>87</v>
       </c>
@@ -3529,7 +3532,7 @@
     </row>
     <row r="8" spans="1:8" ht="79.2">
       <c r="A8" s="119"/>
-      <c r="B8" s="122"/>
+      <c r="B8" s="121"/>
       <c r="C8" s="39" t="s">
         <v>88</v>
       </c>
@@ -3551,7 +3554,7 @@
     </row>
     <row r="9" spans="1:8" ht="26.4">
       <c r="A9" s="119"/>
-      <c r="B9" s="122"/>
+      <c r="B9" s="121"/>
       <c r="C9" s="45" t="s">
         <v>86</v>
       </c>
@@ -3575,7 +3578,7 @@
       <c r="A10" s="118">
         <v>2</v>
       </c>
-      <c r="B10" s="121" t="s">
+      <c r="B10" s="120" t="s">
         <v>89</v>
       </c>
       <c r="C10" s="47" t="s">
@@ -3599,7 +3602,7 @@
     </row>
     <row r="11" spans="1:8" ht="132">
       <c r="A11" s="119"/>
-      <c r="B11" s="122"/>
+      <c r="B11" s="121"/>
       <c r="C11" s="5" t="s">
         <v>91</v>
       </c>
@@ -3621,7 +3624,7 @@
     </row>
     <row r="12" spans="1:8" ht="79.2">
       <c r="A12" s="119"/>
-      <c r="B12" s="122"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="39" t="s">
         <v>92</v>
       </c>
@@ -3643,7 +3646,7 @@
     </row>
     <row r="13" spans="1:8" ht="26.4">
       <c r="A13" s="119"/>
-      <c r="B13" s="122"/>
+      <c r="B13" s="121"/>
       <c r="C13" s="39" t="s">
         <v>86</v>
       </c>
@@ -3667,7 +3670,7 @@
       <c r="A14" s="118">
         <v>3</v>
       </c>
-      <c r="B14" s="121" t="s">
+      <c r="B14" s="120" t="s">
         <v>93</v>
       </c>
       <c r="C14" s="48" t="s">
@@ -3691,7 +3694,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="119"/>
-      <c r="B15" s="122"/>
+      <c r="B15" s="121"/>
       <c r="C15" s="47" t="s">
         <v>90</v>
       </c>
@@ -3711,7 +3714,7 @@
     </row>
     <row r="16" spans="1:8" ht="39.6">
       <c r="A16" s="119"/>
-      <c r="B16" s="122"/>
+      <c r="B16" s="121"/>
       <c r="C16" s="47" t="s">
         <v>95</v>
       </c>
@@ -3733,7 +3736,7 @@
     </row>
     <row r="17" spans="1:8" ht="79.2">
       <c r="A17" s="119"/>
-      <c r="B17" s="122"/>
+      <c r="B17" s="121"/>
       <c r="C17" s="39" t="s">
         <v>96</v>
       </c>
@@ -3755,7 +3758,7 @@
     </row>
     <row r="18" spans="1:8" ht="52.8">
       <c r="A18" s="119"/>
-      <c r="B18" s="122"/>
+      <c r="B18" s="121"/>
       <c r="C18" s="39" t="s">
         <v>97</v>
       </c>
@@ -3777,7 +3780,7 @@
     </row>
     <row r="19" spans="1:8" ht="26.4">
       <c r="A19" s="119"/>
-      <c r="B19" s="122"/>
+      <c r="B19" s="121"/>
       <c r="C19" s="39" t="s">
         <v>86</v>
       </c>
@@ -3801,7 +3804,7 @@
       <c r="A20" s="118">
         <v>4</v>
       </c>
-      <c r="B20" s="121" t="s">
+      <c r="B20" s="120" t="s">
         <v>98</v>
       </c>
       <c r="C20" s="47" t="s">
@@ -3825,7 +3828,7 @@
     </row>
     <row r="21" spans="1:8" ht="39.6">
       <c r="A21" s="119"/>
-      <c r="B21" s="122"/>
+      <c r="B21" s="121"/>
       <c r="C21" s="47" t="s">
         <v>99</v>
       </c>
@@ -3847,7 +3850,7 @@
     </row>
     <row r="22" spans="1:8" ht="79.2">
       <c r="A22" s="119"/>
-      <c r="B22" s="122"/>
+      <c r="B22" s="121"/>
       <c r="C22" s="39" t="s">
         <v>100</v>
       </c>
@@ -3869,7 +3872,7 @@
     </row>
     <row r="23" spans="1:8" ht="52.8">
       <c r="A23" s="119"/>
-      <c r="B23" s="122"/>
+      <c r="B23" s="121"/>
       <c r="C23" s="39" t="s">
         <v>101</v>
       </c>
@@ -3891,7 +3894,7 @@
     </row>
     <row r="24" spans="1:8" ht="26.4">
       <c r="A24" s="119"/>
-      <c r="B24" s="122"/>
+      <c r="B24" s="121"/>
       <c r="C24" s="39" t="s">
         <v>86</v>
       </c>
@@ -3915,7 +3918,7 @@
       <c r="A25" s="118">
         <v>5</v>
       </c>
-      <c r="B25" s="121" t="s">
+      <c r="B25" s="120" t="s">
         <v>102</v>
       </c>
       <c r="C25" s="47" t="s">
@@ -3939,7 +3942,7 @@
     </row>
     <row r="26" spans="1:8" ht="79.2">
       <c r="A26" s="119"/>
-      <c r="B26" s="122"/>
+      <c r="B26" s="121"/>
       <c r="C26" s="49" t="s">
         <v>103</v>
       </c>
@@ -3961,7 +3964,7 @@
     </row>
     <row r="27" spans="1:8" ht="26.4">
       <c r="A27" s="119"/>
-      <c r="B27" s="122"/>
+      <c r="B27" s="121"/>
       <c r="C27" s="3" t="s">
         <v>105</v>
       </c>
@@ -3983,7 +3986,7 @@
     </row>
     <row r="28" spans="1:8" ht="79.2">
       <c r="A28" s="119"/>
-      <c r="B28" s="122"/>
+      <c r="B28" s="121"/>
       <c r="C28" s="39" t="s">
         <v>106</v>
       </c>
@@ -4005,7 +4008,7 @@
     </row>
     <row r="29" spans="1:8" ht="26.4">
       <c r="A29" s="119"/>
-      <c r="B29" s="122"/>
+      <c r="B29" s="121"/>
       <c r="C29" s="39" t="s">
         <v>86</v>
       </c>
@@ -4029,7 +4032,7 @@
       <c r="A30" s="118">
         <v>6</v>
       </c>
-      <c r="B30" s="121" t="s">
+      <c r="B30" s="120" t="s">
         <v>107</v>
       </c>
       <c r="C30" s="47" t="s">
@@ -4163,7 +4166,7 @@
       <c r="A36" s="118">
         <v>7</v>
       </c>
-      <c r="B36" s="121" t="s">
+      <c r="B36" s="120" t="s">
         <v>110</v>
       </c>
       <c r="C36" s="34" t="s">
@@ -4187,7 +4190,7 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="119"/>
-      <c r="B37" s="122"/>
+      <c r="B37" s="121"/>
       <c r="C37" s="48" t="s">
         <v>111</v>
       </c>
@@ -4209,7 +4212,7 @@
     </row>
     <row r="38" spans="1:8" ht="39.6">
       <c r="A38" s="119"/>
-      <c r="B38" s="122"/>
+      <c r="B38" s="121"/>
       <c r="C38" s="50" t="s">
         <v>160</v>
       </c>
@@ -4231,7 +4234,7 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="119"/>
-      <c r="B39" s="122"/>
+      <c r="B39" s="121"/>
       <c r="C39" s="50" t="s">
         <v>159</v>
       </c>
@@ -4253,7 +4256,7 @@
     </row>
     <row r="40" spans="1:8" ht="52.8">
       <c r="A40" s="119"/>
-      <c r="B40" s="122"/>
+      <c r="B40" s="121"/>
       <c r="C40" s="39" t="s">
         <v>112</v>
       </c>
@@ -4275,7 +4278,7 @@
     </row>
     <row r="41" spans="1:8" ht="26.4">
       <c r="A41" s="119"/>
-      <c r="B41" s="122"/>
+      <c r="B41" s="121"/>
       <c r="C41" s="39" t="s">
         <v>86</v>
       </c>
@@ -4299,7 +4302,7 @@
       <c r="A42" s="118">
         <v>8</v>
       </c>
-      <c r="B42" s="121" t="s">
+      <c r="B42" s="120" t="s">
         <v>113</v>
       </c>
       <c r="C42" s="34" t="s">
@@ -4323,7 +4326,7 @@
     </row>
     <row r="43" spans="1:8" ht="52.8">
       <c r="A43" s="119"/>
-      <c r="B43" s="122"/>
+      <c r="B43" s="121"/>
       <c r="C43" s="50" t="s">
         <v>161</v>
       </c>
@@ -4345,7 +4348,7 @@
     </row>
     <row r="44" spans="1:8" ht="39.6">
       <c r="A44" s="119"/>
-      <c r="B44" s="122"/>
+      <c r="B44" s="121"/>
       <c r="C44" s="50" t="s">
         <v>162</v>
       </c>
@@ -4367,7 +4370,7 @@
     </row>
     <row r="45" spans="1:8" ht="52.8">
       <c r="A45" s="119"/>
-      <c r="B45" s="122"/>
+      <c r="B45" s="121"/>
       <c r="C45" s="39" t="s">
         <v>114</v>
       </c>
@@ -4389,7 +4392,7 @@
     </row>
     <row r="46" spans="1:8" ht="26.4">
       <c r="A46" s="119"/>
-      <c r="B46" s="122"/>
+      <c r="B46" s="121"/>
       <c r="C46" s="39" t="s">
         <v>86</v>
       </c>
@@ -4413,7 +4416,7 @@
       <c r="A47" s="118">
         <v>9</v>
       </c>
-      <c r="B47" s="121" t="s">
+      <c r="B47" s="120" t="s">
         <v>115</v>
       </c>
       <c r="C47" s="34" t="s">
@@ -4437,7 +4440,7 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="119"/>
-      <c r="B48" s="122"/>
+      <c r="B48" s="121"/>
       <c r="C48" s="48" t="s">
         <v>116</v>
       </c>
@@ -4459,7 +4462,7 @@
     </row>
     <row r="49" spans="1:10" ht="57" customHeight="1">
       <c r="A49" s="119"/>
-      <c r="B49" s="122"/>
+      <c r="B49" s="121"/>
       <c r="C49" s="50" t="s">
         <v>163</v>
       </c>
@@ -4481,7 +4484,7 @@
     </row>
     <row r="50" spans="1:10" ht="39.6">
       <c r="A50" s="119"/>
-      <c r="B50" s="122"/>
+      <c r="B50" s="121"/>
       <c r="C50" s="50" t="s">
         <v>164</v>
       </c>
@@ -4503,7 +4506,7 @@
     </row>
     <row r="51" spans="1:10" ht="52.8">
       <c r="A51" s="119"/>
-      <c r="B51" s="122"/>
+      <c r="B51" s="121"/>
       <c r="C51" s="39" t="s">
         <v>117</v>
       </c>
@@ -4525,7 +4528,7 @@
     </row>
     <row r="52" spans="1:10" ht="26.4">
       <c r="A52" s="119"/>
-      <c r="B52" s="122"/>
+      <c r="B52" s="121"/>
       <c r="C52" s="39" t="s">
         <v>86</v>
       </c>
@@ -4549,7 +4552,7 @@
       <c r="A53" s="118">
         <v>10</v>
       </c>
-      <c r="B53" s="121" t="s">
+      <c r="B53" s="120" t="s">
         <v>118</v>
       </c>
       <c r="C53" s="34" t="s">
@@ -4573,7 +4576,7 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="119"/>
-      <c r="B54" s="122"/>
+      <c r="B54" s="121"/>
       <c r="C54" s="49" t="s">
         <v>118</v>
       </c>
@@ -4595,7 +4598,7 @@
     </row>
     <row r="55" spans="1:10" ht="79.2">
       <c r="A55" s="119"/>
-      <c r="B55" s="122"/>
+      <c r="B55" s="121"/>
       <c r="C55" s="39" t="s">
         <v>119</v>
       </c>
@@ -4617,7 +4620,7 @@
     </row>
     <row r="56" spans="1:10" ht="13.8">
       <c r="A56" s="119"/>
-      <c r="B56" s="122"/>
+      <c r="B56" s="121"/>
       <c r="C56" s="39" t="s">
         <v>165</v>
       </c>
@@ -4639,7 +4642,7 @@
     </row>
     <row r="57" spans="1:10" ht="52.8">
       <c r="A57" s="119"/>
-      <c r="B57" s="122"/>
+      <c r="B57" s="121"/>
       <c r="C57" s="39" t="s">
         <v>120</v>
       </c>
@@ -4661,7 +4664,7 @@
     </row>
     <row r="58" spans="1:10" ht="26.4">
       <c r="A58" s="119"/>
-      <c r="B58" s="122"/>
+      <c r="B58" s="121"/>
       <c r="C58" s="39" t="s">
         <v>86</v>
       </c>
@@ -4685,7 +4688,7 @@
       <c r="A59" s="118">
         <v>11</v>
       </c>
-      <c r="B59" s="121" t="s">
+      <c r="B59" s="120" t="s">
         <v>121</v>
       </c>
       <c r="C59" s="54" t="s">
@@ -4709,7 +4712,7 @@
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="119"/>
-      <c r="B60" s="122"/>
+      <c r="B60" s="121"/>
       <c r="C60" s="48" t="s">
         <v>122</v>
       </c>
@@ -4732,7 +4735,7 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="119"/>
-      <c r="B61" s="122"/>
+      <c r="B61" s="121"/>
       <c r="C61" s="49" t="s">
         <v>121</v>
       </c>
@@ -4754,7 +4757,7 @@
     </row>
     <row r="62" spans="1:10" ht="26.4">
       <c r="A62" s="119"/>
-      <c r="B62" s="122"/>
+      <c r="B62" s="121"/>
       <c r="C62" s="39" t="s">
         <v>123</v>
       </c>
@@ -4776,7 +4779,7 @@
     </row>
     <row r="63" spans="1:10" ht="26.4">
       <c r="A63" s="119"/>
-      <c r="B63" s="122"/>
+      <c r="B63" s="121"/>
       <c r="C63" s="39" t="s">
         <v>124</v>
       </c>
@@ -4798,7 +4801,7 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="119"/>
-      <c r="B64" s="122"/>
+      <c r="B64" s="121"/>
       <c r="C64" s="55" t="s">
         <v>125</v>
       </c>
@@ -4819,8 +4822,8 @@
       </c>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="120"/>
-      <c r="B65" s="123"/>
+      <c r="A65" s="125"/>
+      <c r="B65" s="126"/>
       <c r="C65" s="55" t="s">
         <v>18</v>
       </c>
@@ -4891,7 +4894,7 @@
       </c>
     </row>
     <row r="68" spans="1:8" ht="15" customHeight="1">
-      <c r="A68" s="120"/>
+      <c r="A68" s="125"/>
       <c r="B68" s="74"/>
       <c r="C68" s="49" t="s">
         <v>130</v>
@@ -4915,22 +4918,6 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="25">
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="A36:A41"/>
-    <mergeCell ref="B36:B41"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="B25:B29"/>
     <mergeCell ref="A59:A65"/>
     <mergeCell ref="A66:A68"/>
     <mergeCell ref="A42:A46"/>
@@ -4940,6 +4927,22 @@
     <mergeCell ref="A53:A58"/>
     <mergeCell ref="B53:B58"/>
     <mergeCell ref="B59:B65"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="A36:A41"/>
+    <mergeCell ref="B36:B41"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="B3:B9"/>
   </mergeCells>
   <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -5118,9 +5121,9 @@
         <f>AND(Syllabus!B5,"AAAAAH7b/yI=")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AJ1" t="b">
+      <c r="AJ1" t="e">
         <f>AND(Syllabus!C5,"AAAAAH7b/yM=")</f>
-        <v>1</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AK1" t="e">
         <f>AND(Syllabus!D5,"AAAAAH7b/yQ=")</f>

</xml_diff>

<commit_message>
update return status when import duplicate (#116)
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/Template_Import_Syllabus.xlsx
+++ b/src/main/resources/templates/Template_Import_Syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSA\Project\fms-backend-api\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1288C0CB-C690-4188-9686-F8FD6BB9DC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5D4FFC-735B-4545-910D-BB24F1142922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -375,7 +375,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="175">
   <si>
     <t>Topic Name</t>
   </si>
@@ -971,6 +971,9 @@
   </si>
   <si>
     <t>TEEST</t>
+  </si>
+  <si>
+    <t>4.1</t>
   </si>
 </sst>
 </file>
@@ -1855,26 +1858,26 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -2907,7 +2910,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:F5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
@@ -2984,8 +2987,8 @@
       <c r="B5" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="115">
-        <v>49</v>
+      <c r="C5" s="115" t="s">
+        <v>174</v>
       </c>
       <c r="D5" s="116"/>
       <c r="E5" s="116"/>
@@ -3377,23 +3380,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36.75" customHeight="1">
-      <c r="A1" s="124" t="str">
+      <c r="A1" s="122" t="str">
         <f>Syllabus!C3 &amp; " - Training Schedule"</f>
         <v>TEST - Training Schedule</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
     </row>
     <row r="2" spans="1:8" ht="39" customHeight="1">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="126"/>
+      <c r="B2" s="124"/>
       <c r="C2" s="31" t="s">
         <v>13</v>
       </c>
@@ -3417,7 +3420,7 @@
       <c r="A3" s="118">
         <v>1</v>
       </c>
-      <c r="B3" s="121" t="s">
+      <c r="B3" s="120" t="s">
         <v>81</v>
       </c>
       <c r="C3" s="34" t="s">
@@ -3441,7 +3444,7 @@
     </row>
     <row r="4" spans="1:8" ht="79.2">
       <c r="A4" s="119"/>
-      <c r="B4" s="122"/>
+      <c r="B4" s="121"/>
       <c r="C4" s="5" t="s">
         <v>84</v>
       </c>
@@ -3463,7 +3466,7 @@
     </row>
     <row r="5" spans="1:8" ht="79.2">
       <c r="A5" s="119"/>
-      <c r="B5" s="122"/>
+      <c r="B5" s="121"/>
       <c r="C5" s="39" t="s">
         <v>85</v>
       </c>
@@ -3485,7 +3488,7 @@
     </row>
     <row r="6" spans="1:8" ht="26.4">
       <c r="A6" s="119"/>
-      <c r="B6" s="122"/>
+      <c r="B6" s="121"/>
       <c r="C6" s="39" t="s">
         <v>86</v>
       </c>
@@ -3507,7 +3510,7 @@
     </row>
     <row r="7" spans="1:8" ht="158.4">
       <c r="A7" s="119"/>
-      <c r="B7" s="122"/>
+      <c r="B7" s="121"/>
       <c r="C7" s="40" t="s">
         <v>87</v>
       </c>
@@ -3529,7 +3532,7 @@
     </row>
     <row r="8" spans="1:8" ht="79.2">
       <c r="A8" s="119"/>
-      <c r="B8" s="122"/>
+      <c r="B8" s="121"/>
       <c r="C8" s="39" t="s">
         <v>88</v>
       </c>
@@ -3551,7 +3554,7 @@
     </row>
     <row r="9" spans="1:8" ht="26.4">
       <c r="A9" s="119"/>
-      <c r="B9" s="122"/>
+      <c r="B9" s="121"/>
       <c r="C9" s="45" t="s">
         <v>86</v>
       </c>
@@ -3575,7 +3578,7 @@
       <c r="A10" s="118">
         <v>2</v>
       </c>
-      <c r="B10" s="121" t="s">
+      <c r="B10" s="120" t="s">
         <v>89</v>
       </c>
       <c r="C10" s="47" t="s">
@@ -3599,7 +3602,7 @@
     </row>
     <row r="11" spans="1:8" ht="132">
       <c r="A11" s="119"/>
-      <c r="B11" s="122"/>
+      <c r="B11" s="121"/>
       <c r="C11" s="5" t="s">
         <v>91</v>
       </c>
@@ -3621,7 +3624,7 @@
     </row>
     <row r="12" spans="1:8" ht="79.2">
       <c r="A12" s="119"/>
-      <c r="B12" s="122"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="39" t="s">
         <v>92</v>
       </c>
@@ -3643,7 +3646,7 @@
     </row>
     <row r="13" spans="1:8" ht="26.4">
       <c r="A13" s="119"/>
-      <c r="B13" s="122"/>
+      <c r="B13" s="121"/>
       <c r="C13" s="39" t="s">
         <v>86</v>
       </c>
@@ -3667,7 +3670,7 @@
       <c r="A14" s="118">
         <v>3</v>
       </c>
-      <c r="B14" s="121" t="s">
+      <c r="B14" s="120" t="s">
         <v>93</v>
       </c>
       <c r="C14" s="48" t="s">
@@ -3691,7 +3694,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="119"/>
-      <c r="B15" s="122"/>
+      <c r="B15" s="121"/>
       <c r="C15" s="47" t="s">
         <v>90</v>
       </c>
@@ -3711,7 +3714,7 @@
     </row>
     <row r="16" spans="1:8" ht="39.6">
       <c r="A16" s="119"/>
-      <c r="B16" s="122"/>
+      <c r="B16" s="121"/>
       <c r="C16" s="47" t="s">
         <v>95</v>
       </c>
@@ -3733,7 +3736,7 @@
     </row>
     <row r="17" spans="1:8" ht="79.2">
       <c r="A17" s="119"/>
-      <c r="B17" s="122"/>
+      <c r="B17" s="121"/>
       <c r="C17" s="39" t="s">
         <v>96</v>
       </c>
@@ -3755,7 +3758,7 @@
     </row>
     <row r="18" spans="1:8" ht="52.8">
       <c r="A18" s="119"/>
-      <c r="B18" s="122"/>
+      <c r="B18" s="121"/>
       <c r="C18" s="39" t="s">
         <v>97</v>
       </c>
@@ -3777,7 +3780,7 @@
     </row>
     <row r="19" spans="1:8" ht="26.4">
       <c r="A19" s="119"/>
-      <c r="B19" s="122"/>
+      <c r="B19" s="121"/>
       <c r="C19" s="39" t="s">
         <v>86</v>
       </c>
@@ -3801,7 +3804,7 @@
       <c r="A20" s="118">
         <v>4</v>
       </c>
-      <c r="B20" s="121" t="s">
+      <c r="B20" s="120" t="s">
         <v>98</v>
       </c>
       <c r="C20" s="47" t="s">
@@ -3825,7 +3828,7 @@
     </row>
     <row r="21" spans="1:8" ht="39.6">
       <c r="A21" s="119"/>
-      <c r="B21" s="122"/>
+      <c r="B21" s="121"/>
       <c r="C21" s="47" t="s">
         <v>99</v>
       </c>
@@ -3847,7 +3850,7 @@
     </row>
     <row r="22" spans="1:8" ht="79.2">
       <c r="A22" s="119"/>
-      <c r="B22" s="122"/>
+      <c r="B22" s="121"/>
       <c r="C22" s="39" t="s">
         <v>100</v>
       </c>
@@ -3869,7 +3872,7 @@
     </row>
     <row r="23" spans="1:8" ht="52.8">
       <c r="A23" s="119"/>
-      <c r="B23" s="122"/>
+      <c r="B23" s="121"/>
       <c r="C23" s="39" t="s">
         <v>101</v>
       </c>
@@ -3891,7 +3894,7 @@
     </row>
     <row r="24" spans="1:8" ht="26.4">
       <c r="A24" s="119"/>
-      <c r="B24" s="122"/>
+      <c r="B24" s="121"/>
       <c r="C24" s="39" t="s">
         <v>86</v>
       </c>
@@ -3915,7 +3918,7 @@
       <c r="A25" s="118">
         <v>5</v>
       </c>
-      <c r="B25" s="121" t="s">
+      <c r="B25" s="120" t="s">
         <v>102</v>
       </c>
       <c r="C25" s="47" t="s">
@@ -3939,7 +3942,7 @@
     </row>
     <row r="26" spans="1:8" ht="79.2">
       <c r="A26" s="119"/>
-      <c r="B26" s="122"/>
+      <c r="B26" s="121"/>
       <c r="C26" s="49" t="s">
         <v>103</v>
       </c>
@@ -3961,7 +3964,7 @@
     </row>
     <row r="27" spans="1:8" ht="26.4">
       <c r="A27" s="119"/>
-      <c r="B27" s="122"/>
+      <c r="B27" s="121"/>
       <c r="C27" s="3" t="s">
         <v>105</v>
       </c>
@@ -3983,7 +3986,7 @@
     </row>
     <row r="28" spans="1:8" ht="79.2">
       <c r="A28" s="119"/>
-      <c r="B28" s="122"/>
+      <c r="B28" s="121"/>
       <c r="C28" s="39" t="s">
         <v>106</v>
       </c>
@@ -4005,7 +4008,7 @@
     </row>
     <row r="29" spans="1:8" ht="26.4">
       <c r="A29" s="119"/>
-      <c r="B29" s="122"/>
+      <c r="B29" s="121"/>
       <c r="C29" s="39" t="s">
         <v>86</v>
       </c>
@@ -4029,7 +4032,7 @@
       <c r="A30" s="118">
         <v>6</v>
       </c>
-      <c r="B30" s="121" t="s">
+      <c r="B30" s="120" t="s">
         <v>107</v>
       </c>
       <c r="C30" s="47" t="s">
@@ -4163,7 +4166,7 @@
       <c r="A36" s="118">
         <v>7</v>
       </c>
-      <c r="B36" s="121" t="s">
+      <c r="B36" s="120" t="s">
         <v>110</v>
       </c>
       <c r="C36" s="34" t="s">
@@ -4187,7 +4190,7 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="119"/>
-      <c r="B37" s="122"/>
+      <c r="B37" s="121"/>
       <c r="C37" s="48" t="s">
         <v>111</v>
       </c>
@@ -4209,7 +4212,7 @@
     </row>
     <row r="38" spans="1:8" ht="39.6">
       <c r="A38" s="119"/>
-      <c r="B38" s="122"/>
+      <c r="B38" s="121"/>
       <c r="C38" s="50" t="s">
         <v>160</v>
       </c>
@@ -4231,7 +4234,7 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="119"/>
-      <c r="B39" s="122"/>
+      <c r="B39" s="121"/>
       <c r="C39" s="50" t="s">
         <v>159</v>
       </c>
@@ -4253,7 +4256,7 @@
     </row>
     <row r="40" spans="1:8" ht="52.8">
       <c r="A40" s="119"/>
-      <c r="B40" s="122"/>
+      <c r="B40" s="121"/>
       <c r="C40" s="39" t="s">
         <v>112</v>
       </c>
@@ -4275,7 +4278,7 @@
     </row>
     <row r="41" spans="1:8" ht="26.4">
       <c r="A41" s="119"/>
-      <c r="B41" s="122"/>
+      <c r="B41" s="121"/>
       <c r="C41" s="39" t="s">
         <v>86</v>
       </c>
@@ -4299,7 +4302,7 @@
       <c r="A42" s="118">
         <v>8</v>
       </c>
-      <c r="B42" s="121" t="s">
+      <c r="B42" s="120" t="s">
         <v>113</v>
       </c>
       <c r="C42" s="34" t="s">
@@ -4323,7 +4326,7 @@
     </row>
     <row r="43" spans="1:8" ht="52.8">
       <c r="A43" s="119"/>
-      <c r="B43" s="122"/>
+      <c r="B43" s="121"/>
       <c r="C43" s="50" t="s">
         <v>161</v>
       </c>
@@ -4345,7 +4348,7 @@
     </row>
     <row r="44" spans="1:8" ht="39.6">
       <c r="A44" s="119"/>
-      <c r="B44" s="122"/>
+      <c r="B44" s="121"/>
       <c r="C44" s="50" t="s">
         <v>162</v>
       </c>
@@ -4367,7 +4370,7 @@
     </row>
     <row r="45" spans="1:8" ht="52.8">
       <c r="A45" s="119"/>
-      <c r="B45" s="122"/>
+      <c r="B45" s="121"/>
       <c r="C45" s="39" t="s">
         <v>114</v>
       </c>
@@ -4389,7 +4392,7 @@
     </row>
     <row r="46" spans="1:8" ht="26.4">
       <c r="A46" s="119"/>
-      <c r="B46" s="122"/>
+      <c r="B46" s="121"/>
       <c r="C46" s="39" t="s">
         <v>86</v>
       </c>
@@ -4413,7 +4416,7 @@
       <c r="A47" s="118">
         <v>9</v>
       </c>
-      <c r="B47" s="121" t="s">
+      <c r="B47" s="120" t="s">
         <v>115</v>
       </c>
       <c r="C47" s="34" t="s">
@@ -4437,7 +4440,7 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="119"/>
-      <c r="B48" s="122"/>
+      <c r="B48" s="121"/>
       <c r="C48" s="48" t="s">
         <v>116</v>
       </c>
@@ -4459,7 +4462,7 @@
     </row>
     <row r="49" spans="1:10" ht="57" customHeight="1">
       <c r="A49" s="119"/>
-      <c r="B49" s="122"/>
+      <c r="B49" s="121"/>
       <c r="C49" s="50" t="s">
         <v>163</v>
       </c>
@@ -4481,7 +4484,7 @@
     </row>
     <row r="50" spans="1:10" ht="39.6">
       <c r="A50" s="119"/>
-      <c r="B50" s="122"/>
+      <c r="B50" s="121"/>
       <c r="C50" s="50" t="s">
         <v>164</v>
       </c>
@@ -4503,7 +4506,7 @@
     </row>
     <row r="51" spans="1:10" ht="52.8">
       <c r="A51" s="119"/>
-      <c r="B51" s="122"/>
+      <c r="B51" s="121"/>
       <c r="C51" s="39" t="s">
         <v>117</v>
       </c>
@@ -4525,7 +4528,7 @@
     </row>
     <row r="52" spans="1:10" ht="26.4">
       <c r="A52" s="119"/>
-      <c r="B52" s="122"/>
+      <c r="B52" s="121"/>
       <c r="C52" s="39" t="s">
         <v>86</v>
       </c>
@@ -4549,7 +4552,7 @@
       <c r="A53" s="118">
         <v>10</v>
       </c>
-      <c r="B53" s="121" t="s">
+      <c r="B53" s="120" t="s">
         <v>118</v>
       </c>
       <c r="C53" s="34" t="s">
@@ -4573,7 +4576,7 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="119"/>
-      <c r="B54" s="122"/>
+      <c r="B54" s="121"/>
       <c r="C54" s="49" t="s">
         <v>118</v>
       </c>
@@ -4595,7 +4598,7 @@
     </row>
     <row r="55" spans="1:10" ht="79.2">
       <c r="A55" s="119"/>
-      <c r="B55" s="122"/>
+      <c r="B55" s="121"/>
       <c r="C55" s="39" t="s">
         <v>119</v>
       </c>
@@ -4617,7 +4620,7 @@
     </row>
     <row r="56" spans="1:10" ht="13.8">
       <c r="A56" s="119"/>
-      <c r="B56" s="122"/>
+      <c r="B56" s="121"/>
       <c r="C56" s="39" t="s">
         <v>165</v>
       </c>
@@ -4639,7 +4642,7 @@
     </row>
     <row r="57" spans="1:10" ht="52.8">
       <c r="A57" s="119"/>
-      <c r="B57" s="122"/>
+      <c r="B57" s="121"/>
       <c r="C57" s="39" t="s">
         <v>120</v>
       </c>
@@ -4661,7 +4664,7 @@
     </row>
     <row r="58" spans="1:10" ht="26.4">
       <c r="A58" s="119"/>
-      <c r="B58" s="122"/>
+      <c r="B58" s="121"/>
       <c r="C58" s="39" t="s">
         <v>86</v>
       </c>
@@ -4685,7 +4688,7 @@
       <c r="A59" s="118">
         <v>11</v>
       </c>
-      <c r="B59" s="121" t="s">
+      <c r="B59" s="120" t="s">
         <v>121</v>
       </c>
       <c r="C59" s="54" t="s">
@@ -4709,7 +4712,7 @@
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="119"/>
-      <c r="B60" s="122"/>
+      <c r="B60" s="121"/>
       <c r="C60" s="48" t="s">
         <v>122</v>
       </c>
@@ -4732,7 +4735,7 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="119"/>
-      <c r="B61" s="122"/>
+      <c r="B61" s="121"/>
       <c r="C61" s="49" t="s">
         <v>121</v>
       </c>
@@ -4754,7 +4757,7 @@
     </row>
     <row r="62" spans="1:10" ht="26.4">
       <c r="A62" s="119"/>
-      <c r="B62" s="122"/>
+      <c r="B62" s="121"/>
       <c r="C62" s="39" t="s">
         <v>123</v>
       </c>
@@ -4776,7 +4779,7 @@
     </row>
     <row r="63" spans="1:10" ht="26.4">
       <c r="A63" s="119"/>
-      <c r="B63" s="122"/>
+      <c r="B63" s="121"/>
       <c r="C63" s="39" t="s">
         <v>124</v>
       </c>
@@ -4798,7 +4801,7 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="119"/>
-      <c r="B64" s="122"/>
+      <c r="B64" s="121"/>
       <c r="C64" s="55" t="s">
         <v>125</v>
       </c>
@@ -4819,8 +4822,8 @@
       </c>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="120"/>
-      <c r="B65" s="123"/>
+      <c r="A65" s="125"/>
+      <c r="B65" s="126"/>
       <c r="C65" s="55" t="s">
         <v>18</v>
       </c>
@@ -4891,7 +4894,7 @@
       </c>
     </row>
     <row r="68" spans="1:8" ht="15" customHeight="1">
-      <c r="A68" s="120"/>
+      <c r="A68" s="125"/>
       <c r="B68" s="74"/>
       <c r="C68" s="49" t="s">
         <v>130</v>
@@ -4915,22 +4918,6 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="25">
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="A36:A41"/>
-    <mergeCell ref="B36:B41"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="B25:B29"/>
     <mergeCell ref="A59:A65"/>
     <mergeCell ref="A66:A68"/>
     <mergeCell ref="A42:A46"/>
@@ -4940,6 +4927,22 @@
     <mergeCell ref="A53:A58"/>
     <mergeCell ref="B53:B58"/>
     <mergeCell ref="B59:B65"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="A36:A41"/>
+    <mergeCell ref="B36:B41"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="B3:B9"/>
   </mergeCells>
   <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -5118,9 +5121,9 @@
         <f>AND(Syllabus!B5,"AAAAAH7b/yI=")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AJ1" t="b">
+      <c r="AJ1" t="e">
         <f>AND(Syllabus!C5,"AAAAAH7b/yM=")</f>
-        <v>1</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AK1" t="e">
         <f>AND(Syllabus!D5,"AAAAAH7b/yQ=")</f>

</xml_diff>

<commit_message>
update import with training program bug
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/Template_Import_Syllabus.xlsx
+++ b/src/main/resources/templates/Template_Import_Syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSA\Project\fms-backend-api\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5D4FFC-735B-4545-910D-BB24F1142922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17597D11-4C01-4549-A993-A156C2482504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -967,13 +967,13 @@
     <t>TRAINING TOPIC SYLLABUS</t>
   </si>
   <si>
-    <t>TEST</t>
-  </si>
-  <si>
     <t>TEEST</t>
   </si>
   <si>
     <t>4.1</t>
+  </si>
+  <si>
+    <t>TESTthat</t>
   </si>
 </sst>
 </file>
@@ -2910,7 +2910,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C3" sqref="C3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
@@ -2930,7 +2930,7 @@
     <row r="1" spans="1:6" ht="36" customHeight="1">
       <c r="A1" s="104" t="str">
         <f>C3&amp;" "&amp;"Syllabus"</f>
-        <v>TEST Syllabus</v>
+        <v>TESTthat Syllabus</v>
       </c>
       <c r="B1" s="104"/>
       <c r="C1" s="104"/>
@@ -2960,7 +2960,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="112" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D3" s="113"/>
       <c r="E3" s="113"/>
@@ -2974,7 +2974,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="112" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D4" s="113"/>
       <c r="E4" s="113"/>
@@ -2988,7 +2988,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="115" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D5" s="116"/>
       <c r="E5" s="116"/>
@@ -3382,7 +3382,7 @@
     <row r="1" spans="1:8" ht="36.75" customHeight="1">
       <c r="A1" s="122" t="str">
         <f>Syllabus!C3 &amp; " - Training Schedule"</f>
-        <v>TEST - Training Schedule</v>
+        <v>TESTthat - Training Schedule</v>
       </c>
       <c r="B1" s="122"/>
       <c r="C1" s="122"/>

</xml_diff>

<commit_message>
Feature/dathpq2/update import status (#119)
* update return status when import duplicate

* update import with training program bug
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/Template_Import_Syllabus.xlsx
+++ b/src/main/resources/templates/Template_Import_Syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSA\Project\fms-backend-api\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5D4FFC-735B-4545-910D-BB24F1142922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17597D11-4C01-4549-A993-A156C2482504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -967,13 +967,13 @@
     <t>TRAINING TOPIC SYLLABUS</t>
   </si>
   <si>
-    <t>TEST</t>
-  </si>
-  <si>
     <t>TEEST</t>
   </si>
   <si>
     <t>4.1</t>
+  </si>
+  <si>
+    <t>TESTthat</t>
   </si>
 </sst>
 </file>
@@ -2910,7 +2910,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C3" sqref="C3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
@@ -2930,7 +2930,7 @@
     <row r="1" spans="1:6" ht="36" customHeight="1">
       <c r="A1" s="104" t="str">
         <f>C3&amp;" "&amp;"Syllabus"</f>
-        <v>TEST Syllabus</v>
+        <v>TESTthat Syllabus</v>
       </c>
       <c r="B1" s="104"/>
       <c r="C1" s="104"/>
@@ -2960,7 +2960,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="112" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D3" s="113"/>
       <c r="E3" s="113"/>
@@ -2974,7 +2974,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="112" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D4" s="113"/>
       <c r="E4" s="113"/>
@@ -2988,7 +2988,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="115" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D5" s="116"/>
       <c r="E5" s="116"/>
@@ -3382,7 +3382,7 @@
     <row r="1" spans="1:8" ht="36.75" customHeight="1">
       <c r="A1" s="122" t="str">
         <f>Syllabus!C3 &amp; " - Training Schedule"</f>
-        <v>TEST - Training Schedule</v>
+        <v>TESTthat - Training Schedule</v>
       </c>
       <c r="B1" s="122"/>
       <c r="C1" s="122"/>

</xml_diff>